<commit_message>
changes to packing app model
</commit_message>
<xml_diff>
--- a/Packing App Model.xlsx
+++ b/Packing App Model.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="79">
   <si>
     <t>Packing App</t>
   </si>
@@ -186,9 +186,6 @@
     <t>Clothing 3</t>
   </si>
   <si>
-    <t>Clothing on my pack</t>
-  </si>
-  <si>
     <t>Bag of money 1</t>
   </si>
   <si>
@@ -244,6 +241,21 @@
   </si>
   <si>
     <t>Wedding ring</t>
+  </si>
+  <si>
+    <t>Trip Start Date</t>
+  </si>
+  <si>
+    <t>Trip End Date</t>
+  </si>
+  <si>
+    <t>T-shirt</t>
+  </si>
+  <si>
+    <t>Board shorts</t>
+  </si>
+  <si>
+    <t>Clothing on my back</t>
   </si>
 </sst>
 </file>
@@ -299,7 +311,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -341,12 +353,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -367,6 +384,8 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -387,6 +406,8 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -884,7 +905,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>3</v>
       </c>
@@ -898,27 +919,27 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:11">
       <c r="A20">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -929,25 +950,31 @@
         <v>8</v>
       </c>
       <c r="D24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" t="s">
         <v>38</v>
       </c>
-      <c r="E24" t="s">
+      <c r="G24" t="s">
         <v>39</v>
       </c>
-      <c r="F24" t="s">
+      <c r="H24" t="s">
         <v>40</v>
       </c>
-      <c r="G24" t="s">
+      <c r="I24" t="s">
         <v>14</v>
       </c>
-      <c r="H24" t="s">
+      <c r="J24" t="s">
         <v>15</v>
       </c>
-      <c r="I24" t="s">
+      <c r="K24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:11">
       <c r="A25">
         <v>1</v>
       </c>
@@ -957,20 +984,26 @@
       <c r="C25">
         <v>1</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="2">
+        <v>41157</v>
+      </c>
+      <c r="E25" s="2">
+        <v>41197</v>
+      </c>
+      <c r="F25">
         <v>1</v>
       </c>
-      <c r="E25">
+      <c r="G25">
         <v>2</v>
       </c>
-      <c r="G25">
+      <c r="I25">
         <v>30</v>
       </c>
-      <c r="H25">
+      <c r="J25">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:11">
       <c r="A26">
         <v>2</v>
       </c>
@@ -980,46 +1013,58 @@
       <c r="C26">
         <v>2</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="2">
+        <v>41353</v>
+      </c>
+      <c r="E26" s="2">
+        <v>41360</v>
+      </c>
+      <c r="F26">
         <v>3</v>
       </c>
-      <c r="G26">
+      <c r="I26">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:11">
       <c r="A27">
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C27">
         <v>3</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="2">
+        <v>41427</v>
+      </c>
+      <c r="E27" s="2">
+        <v>41431</v>
+      </c>
+      <c r="F27">
         <v>4</v>
       </c>
-      <c r="G27">
+      <c r="I27">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:11">
       <c r="A28">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:11">
       <c r="A29">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:11">
       <c r="A30">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -1073,13 +1118,13 @@
         <v>1</v>
       </c>
       <c r="D34" t="s">
+        <v>78</v>
+      </c>
+      <c r="G34" t="s">
         <v>55</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>56</v>
-      </c>
-      <c r="H34" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -1093,22 +1138,28 @@
         <v>2</v>
       </c>
       <c r="D35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" t="s">
+        <v>76</v>
+      </c>
+      <c r="F35" t="s">
+        <v>77</v>
+      </c>
+      <c r="G35" t="s">
+        <v>59</v>
+      </c>
+      <c r="H35" t="s">
         <v>58</v>
       </c>
-      <c r="G35" t="s">
+      <c r="I35" t="s">
+        <v>61</v>
+      </c>
+      <c r="J35" t="s">
         <v>60</v>
       </c>
-      <c r="H35" t="s">
-        <v>59</v>
-      </c>
-      <c r="I35" t="s">
-        <v>62</v>
-      </c>
-      <c r="J35" t="s">
-        <v>61</v>
-      </c>
       <c r="K35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -1122,31 +1173,31 @@
         <v>3</v>
       </c>
       <c r="D36" t="s">
+        <v>64</v>
+      </c>
+      <c r="E36" t="s">
         <v>65</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>66</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>67</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
+        <v>73</v>
+      </c>
+      <c r="I36" t="s">
         <v>68</v>
       </c>
-      <c r="H36" t="s">
-        <v>74</v>
-      </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>69</v>
       </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
         <v>70</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
         <v>71</v>
-      </c>
-      <c r="L36" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:12">

</xml_diff>